<commit_message>
Beautify model name in prediction plot.
</commit_message>
<xml_diff>
--- a/evaluation/results.xlsx
+++ b/evaluation/results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameenislam/Documents/MSc_Project/code.nosync/chbmit-seizure-prediction/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4304AD6-092C-7748-B816-4583EDADC00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A02489-209A-884F-BABD-299905520CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{854A9016-B9AF-B343-B0B6-05CC0D2DDAEC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="19900" activeTab="1" xr2:uid="{854A9016-B9AF-B343-B0B6-05CC0D2DDAEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Patient</t>
   </si>
@@ -76,6 +77,63 @@
   </si>
   <si>
     <t>Total Hours</t>
+  </si>
+  <si>
+    <t>chb01_ARMA_Linear_SVM_v2</t>
+  </si>
+  <si>
+    <t>chb01_ARMA_Linear_SVM_v2 MA</t>
+  </si>
+  <si>
+    <t>Ground Truth</t>
+  </si>
+  <si>
+    <t>0-0.25</t>
+  </si>
+  <si>
+    <t>0.25-0.5</t>
+  </si>
+  <si>
+    <t>Time Interval</t>
+  </si>
+  <si>
+    <t>0.5-0.75</t>
+  </si>
+  <si>
+    <t>0.75-1</t>
+  </si>
+  <si>
+    <t>1-1.25</t>
+  </si>
+  <si>
+    <t>1.25-1.5</t>
+  </si>
+  <si>
+    <t>1.5-1.75</t>
+  </si>
+  <si>
+    <t>1.75-2</t>
+  </si>
+  <si>
+    <t>2-2.25</t>
+  </si>
+  <si>
+    <t>2.25-2.5</t>
+  </si>
+  <si>
+    <t>2.5-2.75</t>
+  </si>
+  <si>
+    <t>2.75-3</t>
+  </si>
+  <si>
+    <t>3-3.25</t>
+  </si>
+  <si>
+    <t>3.25-3.5</t>
+  </si>
+  <si>
+    <t>3.5-3.75</t>
   </si>
 </sst>
 </file>
@@ -125,6 +183,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -133,10 +195,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -460,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB143940-BB8D-6B45-81EC-CF406BCAE1F0}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,7 +543,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -497,95 +555,95 @@
       <c r="D1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2" t="s">
+      <c r="N2" s="4"/>
+      <c r="O2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="2"/>
+      <c r="P2" s="4"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -633,19 +691,192 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="E2:F2"/>
     <mergeCell ref="E1:J1"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="K1:P1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71D8512-E0F4-864F-9917-8BD200511B6C}">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+      <c r="H2">
+        <v>-1</v>
+      </c>
+      <c r="I2">
+        <v>-1</v>
+      </c>
+      <c r="J2">
+        <v>-1</v>
+      </c>
+      <c r="K2">
+        <v>-1</v>
+      </c>
+      <c r="L2">
+        <v>-1</v>
+      </c>
+      <c r="M2">
+        <v>-1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>-1</v>
+      </c>
+      <c r="M3">
+        <v>-1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>